<commit_message>
initial state created and printed
</commit_message>
<xml_diff>
--- a/resources/Amoozesh.xlsx
+++ b/resources/Amoozesh.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alireza/PycharmProjects/uctp/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amirhosseinrahimi/PycharmProjects/TimeTableing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{38FAEAB7-89F8-5E47-BF24-134F12501AA6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -69,9 +68,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -363,11 +359,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:XFD1048576"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>